<commit_message>
Fixed time embedding in LSTM agent
</commit_message>
<xml_diff>
--- a/experiments/pg/return_discount_increment/test/oracle_buffer.xlsx
+++ b/experiments/pg/return_discount_increment/test/oracle_buffer.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3318"/>
+  <dimension ref="A1:C3321"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -43566,6 +43566,45 @@
         <v>13.93145775337879</v>
       </c>
     </row>
+    <row r="3319">
+      <c r="A3319" s="1" t="n">
+        <v>3317</v>
+      </c>
+      <c r="B3319" t="inlineStr">
+        <is>
+          <t>[-6, 7, 7]</t>
+        </is>
+      </c>
+      <c r="C3319" t="n">
+        <v>13.95055801933671</v>
+      </c>
+    </row>
+    <row r="3320">
+      <c r="A3320" s="1" t="n">
+        <v>3318</v>
+      </c>
+      <c r="B3320" t="inlineStr">
+        <is>
+          <t>[-7, 7, 7]</t>
+        </is>
+      </c>
+      <c r="C3320" t="n">
+        <v>13.93074106910142</v>
+      </c>
+    </row>
+    <row r="3321">
+      <c r="A3321" s="1" t="n">
+        <v>3319</v>
+      </c>
+      <c r="B3321" t="inlineStr">
+        <is>
+          <t>[-7, 7, 6]</t>
+        </is>
+      </c>
+      <c r="C3321" t="n">
+        <v>13.93420312523307</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>